<commit_message>
Works now, added 20 shot pool, Refactor experiment configuration and prompts; remove demo files and add startup script,
</commit_message>
<xml_diff>
--- a/data/tickets_examples.xlsx
+++ b/data/tickets_examples.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteoise/Documents/Academic/Projects/Projektarbeit 2/Data/simple/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteoise/Documents/Development/Projects/few-shot-classification-experiment/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF720C32-813A-FF4D-ADEE-07C64C53C675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3992D81E-DD1B-8041-AF56-4640395352F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{37832037-8207-C04A-9214-B0842A5D6D68}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'aa_dataset-tickets-multi-lang-5'!$A$1:$I$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'aa_dataset-tickets-multi-lang-5'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="84">
   <si>
     <t>subject</t>
   </si>
@@ -95,21 +95,9 @@
     <t>Security</t>
   </si>
   <si>
-    <t>Account Disruption</t>
-  </si>
-  <si>
-    <t>Dear Customer Support Team,\n\nI am writing to report a significant problem with the centralized account management portal, which currently appears to be offline. This outage is blocking access to account settings, leading to substantial inconvenience. I have attempted to log in multiple times using different browsers and devices, but the issue persists.\n\nCould you please provide an update on the outage status and an estimated time for resolution? Also, are there any alternative ways to access and manage my account during this downtime?</t>
-  </si>
-  <si>
-    <t>Thank you for reaching out, &lt;name&gt;. We are aware of the outage affecting the centralized account management system, and our technical team is actively working to resolve the issue. In the meantime, we suggest using alternative methods to manage your account, with a focus on restoring service as quickly as possible. We will provide an update as soon as the service is back online. We apologize for the inconvenience and appreciate your patience. If you have any further questions, please let us know.</t>
-  </si>
-  <si>
     <t>en</t>
   </si>
   <si>
-    <t>Account</t>
-  </si>
-  <si>
     <t>medium</t>
   </si>
   <si>
@@ -156,6 +144,162 @@
   </si>
   <si>
     <t>label</t>
+  </si>
+  <si>
+    <t>Audio Hardware Detected</t>
+  </si>
+  <si>
+    <t>Dear Customer Support Team,\n\nI am reaching out to request help with a problem I am facing on my PC. Recently, the audio hardware is no longer being recognized by the system. Despite several troubleshooting efforts, such as reconnecting the device, updating the drivers, and restarting the computer, the issue persists. This problem has made the audio output completely unusable, impacting my ability to listen to media and participate in video calls.\n\nI have checked the Device Manager, and the audio hardware appears in the list of devices, with the connections confirmed.</t>
+  </si>
+  <si>
+    <t>Thank you for reaching out to us, &lt;name&gt;. Since the audio hardware is detected in Device Manager and drivers have been updated and the system restarted, please ensure the device is securely connected and try using a different port or cable. If you have a removable audio card, reseat it if possible. If these steps help, please let us know the specific model of your audio device, whether it is built-in or external, so we can provide more targeted assistance.</t>
+  </si>
+  <si>
+    <t>Problem</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>SSD-Ausfall</t>
+  </si>
+  <si>
+    <t>Sehr geehrter Kundendienst,\n\nich erfahre wiederholte Fehler bei der Datenübertragung mit meiner Crucial MX500 1TB SSD. Das Problem trat kürzlich nach einem Betriebssystem-Update auf und scheint auf Kompatibilitätsprobleme hinzuweisen. Ich habe bereits mehrere Schritte zur Fehlerbehebung unternommen, darunter den Neustart des Computers, ein Firmware-Update der SSD, den Austausch des Datenkabels, doch das Problem besteht weiterhin. Die Übertragung stoppt entweder abrupt, schlägt fehl oder kann nicht erfolgreich abgeschlossen werden. Könnten Sie bitte bei der Diagnose und Lösung des Problems behilflich sein? Eine Anleitung zu empfohlenen Maßnahmen wäre sehr hilfreich.</t>
+  </si>
+  <si>
+    <t>Vielen Dank, dass Sie sich wegen des Problems mit Ihrer Crucial MX500 SSD an uns gewandt haben. Um Ihnen bestmöglich weiterhelfen zu können, teilen Sie uns bitte die Version Ihres Betriebssystems mit sowie Informationen darüber, ob die SSD intern installiert oder in einem externen Gehäuse verwendet wird. Falls vorhanden, geben Sie bitte auch spezifische Fehlermeldungen an, die bei den fehlgeschlagenen Übertragungen erscheinen. Das erleichtert es uns, gezielte Lösungsschritte zur Fehlerbehebung vorzuschlagen.</t>
+  </si>
+  <si>
+    <t>Eiltiges Update für Hardware und Software</t>
+  </si>
+  <si>
+    <t>Sehr geehrter Kundendienst,\n\nich bitte um sofortige Unterstützung bei Störungen im Hardware- und Software-Service, die kritische Komponenten wie das Motherboard, den CPU-Kühler sowie Netzwerk- und Peripheriegeräte betreffen. Diese Probleme beeinträchtigen wichtige Anwendungen, wobei eine kontinuierliche Geschäfts- und Analysearbeit unerlässlich ist. Eine zügige Lösung ist unbedingt erforderlich, um weitere Störungen im Betriebsablauf zu vermeiden.\n\nVielen Dank im Voraus für die rasche Bearbeitung dieses Anliegens.\n\nMit freundlichen Grüßen,\n[Ihr Name]</t>
+  </si>
+  <si>
+    <t>Sehr geehrter &lt;Name&gt;,\n\nvielen Dank, dass Sie uns wegen der Ausfälle im Hardware- und Software-Service kontaktiert haben. Wir verstehen die Dringlichkeit im Hinblick auf die Auswirkungen auf geschäftskritische Prozesse. Um Ihnen schnellstmöglich zu helfen, könnten Sie bitte zusätzliche Informationen bereitstellen, etwa konkrete Fehlermeldungen, die Modelle der betroffenen Geräte oder kürzliche Änderungen an der Systemumgebung? Falls Warnhinweise bei Ihren Geräten angezeigt werden, lassen Sie uns diese bitte wissen. Außerdem bitten wir um Bestätigung, ob kürzlich System- oder Netzwerksicherungen durchgeführt wurden. Falls ein telefonischer Kontakt zur Fehlerbehebung hilfreich ist, teilen Sie uns dies bitte ebenfalls mit.</t>
+  </si>
+  <si>
+    <t>Service Outages and Maintenance</t>
+  </si>
+  <si>
+    <t>Office Equipment Malfunctions</t>
+  </si>
+  <si>
+    <t>Customer Service Team,\n\nWe are facing concurrent failures in several office gadgets. The problem seems linked to a network disruption causing synchronization issues with cloud services. We've already attempted restarting the devices and checked physical connections, but the issue persists. This disruption is greatly affecting our daily workflow, and we urgently need help to identify and fix the underlying problem. Kindly advise on the next steps and let us know if additional details are required from our side.\n\nThank you.</t>
+  </si>
+  <si>
+    <t>Thank you for reaching out to us. To assist you better, please specify which devices and cloud services are affected, include any error messages you see, and describe the network status indicators. Since this is urgent, inform us of a suitable time for a support call.</t>
+  </si>
+  <si>
+    <t>Connectivity Problems with Printer on MacBook Pro</t>
+  </si>
+  <si>
+    <t>Dear Support Team,\n\nI am reporting a recurring issue with the Laser Printer when printing from MacBook Pros running macOS 15. Several team members have recently encountered this problem, which appears to be connected to the latest macOS 15 system updates.\n\nWe believe the root cause might be a driver compatibility issue due to the updated operating systems or printer firmware. To troubleshoot, we have restarted the printers and MacBook devices, reinstalled the printer drivers, and verified configurations.</t>
+  </si>
+  <si>
+    <t>Thank you for reaching out regarding the connectivity problems with the Laser Printer on MacBook Pros after recent macOS 15 updates. We understand how disruptive this can be and appreciate your efforts in troubleshooting so far. To assist you further, please confirm the specific MacBook model and current macOS version you are using (including whether you have iOS devices like iPhones or iPads). Also, provide the model and driver version of the Laser Printer installed. Meanwhile, we recommend...</t>
+  </si>
+  <si>
+    <t>VPN Access Issue</t>
+  </si>
+  <si>
+    <t>Customer Support,\n\nWe are encountering a disruption in VPN-router connectivity that is impacting several devices, notably essential remote telemedicine systems and EMR integrations. Attempts to resolve the issue by restarting affected devices and resetting the router have been unsuccessful. We suspect the problem may be related to firmware discrepancies following recent network configuration updates. This disruption is significantly affecting our operations, and we urgently need assistance to identify and fix the root cause. Kindly advise on additional troubleshooting steps.</t>
+  </si>
+  <si>
+    <t>Thank you for reporting this problem. Please provide the model of your VPN router, the current firmware version, and details of any recent network modifications. This information will assist us in diagnosing the issue and recommending suitable troubleshooting measures or firmware updates.</t>
+  </si>
+  <si>
+    <t>Product Support</t>
+  </si>
+  <si>
+    <t>Network Connection Problems</t>
+  </si>
+  <si>
+    <t>Dear Customer Support Team,\n\nI am reaching out to report persistent issues with network connectivity that are significantly disrupting my workflow. I've observed sporadic interruptions across several devices, which I believe may be caused by a malfunctioning repeater or potential interference from other devices within the network configuration.\n\nIn an attempt to resolve the problem, I have already taken several measures, such as restarting the affected equipment and repositioning the repeater to different locations within the premises. Despite these efforts, the connectivity issues persist.</t>
+  </si>
+  <si>
+    <t>Thank you for reaching out to us, &lt;name&gt;. We understand the importance of reliable and stable network connectivity. Currently, widespread problems with repeaters and interference in the environment are being reported. To assist you further, could you please specify which devices are impacted, provide details about your network setup, and mention any recent modifications? If possible, kindly share relevant error logs. We are prepared to guide you through advanced troubleshooting procedures.</t>
+  </si>
+  <si>
+    <t>Verbindungsstörung</t>
+  </si>
+  <si>
+    <t>Sehr geehrtes Support-Team,\n\nich möchte ein Verbindungsproblem melden, das meinen Account im Management Hub betrifft. Trotz mehrmaliger Versuche, auf den Hub zuzugreifen, wird die effiziente Verwaltung meines Kontos behindert. Das Problem besteht bereits seit einiger Zeit. Ich habe grundlegende Fehlerbehebungsmaßnahmen wie Neustart des Geräts und Überprüfung der Internetverbindung durchgeführt, jedoch ohne Erfolg. Ich würde eine schnelle Unterstützung bei der Diagnose und Lösung des Problems sehr schätzen, um den vollen Zugriff auf den Management Hub wiederzuerlangen. Bitte informieren Sie mich.</t>
+  </si>
+  <si>
+    <t>Vielen Dank, dass Sie sich wegen der Verbindungsstörung im Account Management Hub an uns gewandt haben. Ich verstehe, dass ein ununterbrochener Zugriff für Sie essenziell ist, und schätze, dass Sie bereits grundlegende Fehlerbehebungen vorgenommen haben. Könnten Sie uns bitte weitere Details zum Fehler mitteilen? Zum Beispiel, erhalten Sie eine bestimmte Fehlermeldung, oder lädt die Seite einfach nicht? Bitte teilen Sie außerdem mit, welches Browser- oder Gerätetyp Sie verwenden und ob das Problem auf mehreren Geräten oder in verschiedenen Netzwerken auftritt.</t>
+  </si>
+  <si>
+    <t>Alert for Unauthorized Entry</t>
+  </si>
+  <si>
+    <t>Dear Customer Support,\n\nI have recently been notified of attempts at unauthorized entry into my IoT gadgets. This has raised significant worries about the security of my home network. I would be grateful for immediate help in examining this issue to ensure my devices are fully secured. Please advise on additional security protocols I can implement and keep me informed about any updates related to this problem. Thank you for your swift response to this urgent security matter.\n\nSincerely,\n[Your Name]</t>
+  </si>
+  <si>
+    <t>We appreciate your reaching out regarding the alert of unauthorized access to your IoT devices. Kindly specify the device models and provide the exact alert details you've received so we can proceed with a thorough investigation. In the meantime, we suggest changing your device passwords, updating their firmware, and enabling two-factor authentication where possible. Feel free to ask for step-by-step guidance on these security measures if needed.</t>
+  </si>
+  <si>
+    <t>Customer Service</t>
+  </si>
+  <si>
+    <t>Critical Security Breach in Telehealth Platforms</t>
+  </si>
+  <si>
+    <t>Dear Customer Support Team,\n\nI am reaching out to urgently highlight a severe security breach impacting our telehealth systems. Recently, we detected abnormal activities that could indicate a security intrusion, potentially jeopardizing confidential patient information and hindering service operations. Due to the vital importance of telehealth services, it is crucial that this issue is addressed without delay.\n\nWe kindly request a comprehensive investigation to determine the root cause and identify any vulnerabilities that may have been exploited. Furthermore, please</t>
+  </si>
+  <si>
+    <t>Thank you for bringing this security concern to our notice. We recognize the urgency of safeguarding sensitive patient information within telehealth platforms. Our security team has initiated an initial review, focusing on pinpointing the underlying vulnerabilities involved. To proceed effectively, could you please share specific details such as the timeframe of the suspicious activity, impacted accounts or systems, and any error messages or logs you have observed? In the meantime, we advise changing administrative passwords and restricting access to essential personnel.</t>
+  </si>
+  <si>
+    <t>Guidance on Secure EMR Integration</t>
+  </si>
+  <si>
+    <t>Dear Customer Support Team,\n\nI am looking for comprehensive instructions on how to securely connect EMR/PACS systems with IoT medical devices and telemedicine platforms. Ensuring this integration aligns with key data privacy and security standards such as HIPAA, GDPR, and ISO 27001 is essential. I would be grateful for recommended practices, protocols, and frameworks that can assist in meeting these compliance requirements efficiently. Furthermore, I seek advice on potential security vulnerabilities and strategies to mitigate associated risks during the integration process.</t>
+  </si>
+  <si>
+    <t>Thank you for reaching out, &lt;name&gt;. For secure EMR/PACS and IoT integrations, it is advisable to adopt standards like HL7/FHIR along with TLS/HTTPS protocols to encrypt data during storage and transmission. Establish robust access controls, conduct regular security audits, and secure endpoints. Utilizing API gateways, identity management solutions, and security tools can help ensure compliance with HIPAA, GDPR, and ISO 27001. Please share your specific system details so we can provide more tailored guidance.</t>
+  </si>
+  <si>
+    <t>Request</t>
+  </si>
+  <si>
+    <t>Advice on Securing Telehealth Platforms</t>
+  </si>
+  <si>
+    <t>Dear Customer Support Team,\n\nI hope this message reaches you well. I am seeking detailed guidance on how to safeguard telehealth systems. As telemedicine becomes an increasingly crucial aspect of healthcare delivery, prioritizing the protection and confidentiality of patient information is essential.\n\nCould you please share comprehensive recommendations and best practices to strengthen the security of telehealth platforms? I am particularly interested in understanding common vulnerabilities these systems face and effective strategies to mitigate potential threats, including the use of encryption.</t>
+  </si>
+  <si>
+    <t>Thank you for reaching out regarding the security of telehealth platforms. To protect patient information and ensure compliance with HIPAA and GDPR, it is important to implement measures such as end-to-end encryption for communications (using TLS 1.2 or higher), enforcing robust user authentication methods (preferably multi-factor authentication), and storing health data in encrypted databases. Regularly updating software and applying security patches promptly, restricting access through role-based permissions, and monitoring system activity for unauthorized access attempts are also vital steps.</t>
+  </si>
+  <si>
+    <t>Assistance with Software and Hardware Integration</t>
+  </si>
+  <si>
+    <t>Dear Customer Support, I am requesting updates on software and hardware integration to improve data analytics and optimize investment strategies for our financial firm. This will help us make better-informed decisions and enhance overall performance. Your support in providing the necessary updates to achieve these goals would be greatly appreciated. Thank you for your time and assistance. I look forward to your prompt response.</t>
+  </si>
+  <si>
+    <t>&lt;name&gt;, thank you for contacting the service desk regarding software and hardware integration updates aimed at enhancing data analytics for your financial firm. We understand the importance of informed decision-making and improving overall efficiency. To assist you more effectively, could you please share details about your current software and hardware configurations, including the specific systems and tools you use for data analytics? Additionally, it would be helpful to know the particular updates you are seeking.</t>
+  </si>
+  <si>
+    <t>Support für Software-Integrationen</t>
+  </si>
+  <si>
+    <t>Sehr geehrter Kundenservice, ich möchte um Aktualisierungen im Bereich Software- und Hardware-Integration bitten, um die Datenanalyse zu optimieren und dadurch unsere Investitionsstrategien bei unserer Finanzfirma zu verbessern. Ihre Unterstützung würde uns helfen, fundiertere Entscheidungen zu treffen und die Gesamtleistung zu steigern. Wir würden es begrüßen, wenn Sie die notwendigen Updates bereitstellen könnten, um unsere Zielsetzung zu erreichen. Vielen Dank für Ihre Zeit und Unterstützung. Wir freuen uns auf eine baldige Rückmeldung.</t>
+  </si>
+  <si>
+    <t>Sehr geehrter &lt;Name&gt;, vielen Dank, dass Sie den Service-Desk bezüglich der Updates zur Software- und Hardware-Integration kontaktiert haben, um die Datenanalyse Ihrer Finanzfirma zu verbessern. Wir verstehen die Bedeutung fundierter Entscheidungen für eine Leistungssteigerung. Um Ihnen besser helfen zu können, bitten wir Sie, weitere Informationen zu Ihrer aktuellen Software- und Hardware-Konfiguration bereitzustellen, einschließlich spezifischer Systeme, Tools und der verwendeten Datenanalyse-Methoden. Zusätzlich wäre es hilfreich zu wissen, welche konkreten Updates Sie benötigen, beispielsweise Schulungen oder Unterstützung bei der Fehlerbehebung bei der Konfiguration. Sobald wir diese Informationen erhalten haben,...</t>
+  </si>
+  <si>
+    <t>Problem with Software Integration</t>
+  </si>
+  <si>
+    <t>Dear Customer Support, I am reporting an issue with the integration of JIRA Software on our scalable SaaS platform. The integration is failing, and we suspect it might be due to a mismatch in API versions. Our team has tried to resolve the problem by updating API keys and restarting services, but unfortunately, the issue remains unresolved. We have attempted multiple times, but the problem persists. We would greatly appreciate your assistance in troubleshooting this matter. Could you please provide us with the current API version?</t>
+  </si>
+  <si>
+    <t>Problems with Digital Tool Integration</t>
+  </si>
+  <si>
+    <t>The marketing agency encountered difficulties integrating digital tools, which impacted their brand growth campaigns. The issues may be due to software conflicts. They have tried troubleshooting by updating individual platform applications but have not succeeded. Assistance is needed to resolve the problem and get the campaigns back on track.</t>
   </si>
 </sst>
 </file>
@@ -565,22 +709,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A029593-E643-EE40-85A6-7B4FB6AC4E1C}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="80.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.6640625" customWidth="1"/>
-    <col min="3" max="3" width="80.6640625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="80.6640625" customWidth="1"/>
     <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" customWidth="1"/>
     <col min="9" max="9" width="89.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -610,178 +754,579 @@
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H2" s="2">
         <v>51</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="2">
+        <v>51</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="H3" s="2">
-        <v>51</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="2">
+        <v>51</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="H4" s="2">
-        <v>51</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="2">
+        <v>51</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="H5" s="2">
-        <v>51</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="2">
+        <v>51</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="2">
+        <v>51</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="2">
+        <v>51</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="2">
+        <v>51</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="2">
+        <v>51</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H11" s="2">
+        <v>51</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="2">
+        <v>51</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="2">
+        <v>51</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="2">
+        <v>51</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="2">
+        <v>51</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="2">
+        <v>51</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="2">
         <v>52</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="I17" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="2">
+        <v>52</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="2">
+        <v>52</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I8" xr:uid="{5A029593-E643-EE40-85A6-7B4FB6AC4E1C}"/>
+  <autoFilter ref="A1:I1" xr:uid="{5A029593-E643-EE40-85A6-7B4FB6AC4E1C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Refactor Status VSCode: Update prompt creation, enhance statistical analysis, and improve visualization quality; add comprehensive documentation on code quality improvements.
</commit_message>
<xml_diff>
--- a/data/tickets_examples.xlsx
+++ b/data/tickets_examples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteoise/Documents/Development/Projects/few-shot-classification-experiment/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D8257B-87B6-7C40-9E06-BD99EB76BBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658EE1E5-10FC-0E4D-937E-C8212E54AB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{37832037-8207-C04A-9214-B0842A5D6D68}"/>
   </bookViews>
@@ -300,7 +300,7 @@
     <t>The marketing agency encountered difficulties integrating digital tools, which impacted their brand growth campaigns. The issues may be due to software conflicts. They have tried troubleshooting by updating individual platform applications but have not succeeded. Assistance is needed to resolve the problem and get the campaigns back on track.</t>
   </si>
   <si>
-    <t>q</t>
+    <t>subject</t>
   </si>
 </sst>
 </file>
@@ -735,9 +735,7 @@
   </sheetPr>
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCellId="1" sqref="I21 A1:I21"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>